<commit_message>
version 2 and 3 plots - preparing for the pa birds paper
</commit_message>
<xml_diff>
--- a/030_data/2020_PA.xlsx
+++ b/030_data/2020_PA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/030_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC705274-1A74-9E44-96E4-9C93438C697D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E9EAED-1191-FF40-B66C-4F1240F39C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="1060" windowWidth="27700" windowHeight="17540" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
+    <workbookView xWindow="1600" yWindow="1760" windowWidth="27700" windowHeight="17540" xr2:uid="{FBB681FB-660C-454A-A7AE-1280157312B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="29">
   <si>
     <t>chicks/nested box</t>
   </si>
@@ -154,14 +154,14 @@
     <t>Emily H. Thomas and Don Watts are based in northwest PA, and a bit into NY state</t>
   </si>
   <si>
-    <t>Central PA Conservancy</t>
+    <t>Central PA Program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +229,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,6 +269,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,16 +584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9474FD0B-C36E-E645-A63D-D7F861907EC9}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -712,40 +720,38 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
+      <c r="A7" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>2022</v>
+      </c>
+      <c r="C7" s="5">
+        <v>646</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4.141</v>
+      </c>
+      <c r="E7" s="5">
+        <v>646</v>
+      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C8" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>19</v>
@@ -756,39 +762,39 @@
         <v>24</v>
       </c>
       <c r="B9" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C9" s="2">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="E9" s="2">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -796,16 +802,16 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C11" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>15</v>
@@ -816,39 +822,39 @@
         <v>21</v>
       </c>
       <c r="B12" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C12" s="2">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="E12" s="2">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="C13" s="2">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="E13" s="2">
-        <v>169</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -856,16 +862,16 @@
         <v>9</v>
       </c>
       <c r="B14" s="2">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="C14" s="2">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D14" s="2">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="E14" s="2">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>16</v>
@@ -876,16 +882,16 @@
         <v>9</v>
       </c>
       <c r="B15" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C15" s="2">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="D15" s="2">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="E15" s="2">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>16</v>
@@ -896,16 +902,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C16" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D16" s="2">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="E16" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>16</v>
@@ -916,13 +922,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C17" s="2">
         <v>208</v>
       </c>
       <c r="D17" s="2">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="E17" s="2">
         <v>208</v>
@@ -936,16 +942,16 @@
         <v>9</v>
       </c>
       <c r="B18" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C18" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D18" s="2">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="E18" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>16</v>
@@ -956,16 +962,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C19" s="2">
-        <v>253</v>
+        <v>206</v>
       </c>
       <c r="D19" s="2">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="E19" s="2">
-        <v>253</v>
+        <v>206</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>16</v>
@@ -973,22 +979,22 @@
     </row>
     <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -996,16 +1002,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C21" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>20</v>
@@ -1016,16 +1022,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C22" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="E22" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>20</v>
@@ -1036,16 +1042,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C23" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D23" s="2">
-        <v>3.7</v>
+        <v>2.4</v>
       </c>
       <c r="E23" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>20</v>
@@ -1056,16 +1062,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C24" s="2">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2">
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="E24" s="2">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>20</v>
@@ -1076,36 +1082,39 @@
         <v>10</v>
       </c>
       <c r="B25" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C25" s="2">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D25" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="2">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
+      <c r="A26" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B26" s="2">
         <v>2020</v>
       </c>
-      <c r="C26" s="4">
-        <v>88</v>
-      </c>
-      <c r="E26" s="4">
-        <v>88</v>
+      <c r="C26" s="2">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>37</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1113,13 +1122,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C27" s="4">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E27" s="4">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>17</v>
@@ -1130,13 +1139,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C28" s="4">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E28" s="4">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>17</v>
@@ -1147,13 +1156,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="2">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C29" s="4">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="E29" s="4">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>17</v>
@@ -1164,13 +1173,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C30" s="4">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="E30" s="4">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>17</v>
@@ -1181,13 +1190,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="2">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C31" s="4">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="E31" s="4">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>17</v>
@@ -1198,13 +1207,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="2">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C32" s="4">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="E32" s="4">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>17</v>
@@ -1215,13 +1224,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="2">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C33" s="4">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="E33" s="4">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>17</v>
@@ -1232,13 +1241,13 @@
         <v>2</v>
       </c>
       <c r="B34" s="2">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C34" s="4">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="E34" s="4">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>17</v>
@@ -1249,13 +1258,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C35" s="4">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="E35" s="4">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>17</v>
@@ -1265,14 +1274,14 @@
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="9">
-        <v>2007</v>
-      </c>
-      <c r="C36" s="9">
-        <v>156</v>
-      </c>
-      <c r="E36" s="9">
-        <v>156</v>
+      <c r="B36" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C36" s="4">
+        <v>183</v>
+      </c>
+      <c r="E36" s="4">
+        <v>183</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>17</v>
@@ -1283,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="9">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C37" s="9">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="E37" s="9">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>17</v>
@@ -1300,13 +1309,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="9">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="C38" s="9">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E38" s="9">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>17</v>
@@ -1317,36 +1326,33 @@
         <v>2</v>
       </c>
       <c r="B39" s="9">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="C39" s="9">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="E39" s="9">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="2">
-        <v>2011</v>
-      </c>
-      <c r="C40" s="2">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2">
-        <v>0</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>26</v>
+    <row r="40" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="9">
+        <v>2010</v>
+      </c>
+      <c r="C40" s="9">
+        <v>207</v>
+      </c>
+      <c r="E40" s="9">
+        <v>207</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1354,16 +1360,16 @@
         <v>25</v>
       </c>
       <c r="B41" s="2">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="C41" s="2">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="E41" s="2">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>26</v>
@@ -1374,16 +1380,16 @@
         <v>25</v>
       </c>
       <c r="B42" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C42" s="2">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D42" s="2">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="E42" s="2">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>26</v>
@@ -1394,16 +1400,16 @@
         <v>25</v>
       </c>
       <c r="B43" s="2">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C43" s="2">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D43" s="2">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="E43" s="2">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>26</v>
@@ -1414,16 +1420,16 @@
         <v>25</v>
       </c>
       <c r="B44" s="2">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="C44" s="2">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D44" s="2">
         <v>2.5</v>
       </c>
       <c r="E44" s="2">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>26</v>
@@ -1434,16 +1440,16 @@
         <v>25</v>
       </c>
       <c r="B45" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C45" s="2">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D45" s="2">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="E45" s="2">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>26</v>
@@ -1454,16 +1460,16 @@
         <v>25</v>
       </c>
       <c r="B46" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C46" s="2">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D46" s="2">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="E46" s="2">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>26</v>
@@ -1474,16 +1480,16 @@
         <v>25</v>
       </c>
       <c r="B47" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C47" s="2">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D47" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="E47" s="2">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>26</v>
@@ -1494,16 +1500,16 @@
         <v>25</v>
       </c>
       <c r="B48" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C48" s="2">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D48" s="2">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E48" s="2">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>26</v>
@@ -1514,36 +1520,39 @@
         <v>25</v>
       </c>
       <c r="B49" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C49" s="2">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="D49" s="2">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="E49" s="2">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="5">
-        <v>2006</v>
+        <v>25</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2020</v>
       </c>
       <c r="C50" s="2">
-        <v>0</v>
+        <v>226</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2.8</v>
       </c>
       <c r="E50" s="2">
-        <v>0</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>22</v>
+        <v>226</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1551,13 +1560,13 @@
         <v>3</v>
       </c>
       <c r="B51" s="5">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C51" s="2">
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="E51" s="2">
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>22</v>
@@ -1568,13 +1577,13 @@
         <v>3</v>
       </c>
       <c r="B52" s="5">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C52" s="2">
-        <v>184</v>
+        <v>264</v>
       </c>
       <c r="E52" s="2">
-        <v>184</v>
+        <v>264</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>22</v>
@@ -1585,13 +1594,13 @@
         <v>3</v>
       </c>
       <c r="B53" s="5">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="C53" s="2">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="E53" s="2">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>22</v>
@@ -1602,13 +1611,13 @@
         <v>3</v>
       </c>
       <c r="B54" s="5">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="C54" s="2">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="E54" s="2">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>22</v>
@@ -1619,13 +1628,13 @@
         <v>3</v>
       </c>
       <c r="B55" s="5">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C55" s="2">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="E55" s="2">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>22</v>
@@ -1636,13 +1645,13 @@
         <v>3</v>
       </c>
       <c r="B56" s="5">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="C56" s="2">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="E56" s="2">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>22</v>
@@ -1653,13 +1662,13 @@
         <v>3</v>
       </c>
       <c r="B57" s="5">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C57" s="2">
-        <v>111</v>
+        <v>183</v>
       </c>
       <c r="E57" s="2">
-        <v>111</v>
+        <v>183</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>22</v>
@@ -1670,13 +1679,13 @@
         <v>3</v>
       </c>
       <c r="B58" s="5">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C58" s="2">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E58" s="2">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>22</v>
@@ -1687,13 +1696,13 @@
         <v>3</v>
       </c>
       <c r="B59" s="5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="C59" s="2">
-        <v>66</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>4</v>
+        <v>126</v>
+      </c>
+      <c r="E59" s="2">
+        <v>126</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>22</v>
@@ -1704,13 +1713,13 @@
         <v>3</v>
       </c>
       <c r="B60" s="5">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C60" s="2">
-        <v>135</v>
-      </c>
-      <c r="E60" s="2">
-        <v>135</v>
+        <v>66</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>22</v>
@@ -1721,13 +1730,13 @@
         <v>3</v>
       </c>
       <c r="B61" s="5">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C61" s="2">
-        <v>85</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>5</v>
+        <v>135</v>
+      </c>
+      <c r="E61" s="2">
+        <v>135</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>22</v>
@@ -1738,13 +1747,13 @@
         <v>3</v>
       </c>
       <c r="B62" s="5">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C62" s="2">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>22</v>
@@ -1755,13 +1764,13 @@
         <v>3</v>
       </c>
       <c r="B63" s="5">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C63" s="2">
-        <v>149</v>
-      </c>
-      <c r="E63" s="2">
-        <v>149</v>
+        <v>93</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>22</v>
@@ -1772,36 +1781,33 @@
         <v>3</v>
       </c>
       <c r="B64" s="5">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C64" s="2">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="E64" s="2">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B65" s="6">
-        <v>2013</v>
-      </c>
-      <c r="C65" s="6">
-        <v>0</v>
-      </c>
-      <c r="D65" s="6">
-        <v>0</v>
-      </c>
-      <c r="E65" s="6">
-        <v>0</v>
+      <c r="A65" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C65" s="2">
+        <v>196</v>
+      </c>
+      <c r="E65" s="2">
+        <v>196</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1809,16 +1815,16 @@
         <v>11</v>
       </c>
       <c r="B66" s="6">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C66" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D66" s="6">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E66" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>18</v>
@@ -1829,16 +1835,16 @@
         <v>11</v>
       </c>
       <c r="B67" s="6">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="C67" s="6">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D67" s="6">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="E67" s="6">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>18</v>
@@ -1849,16 +1855,16 @@
         <v>11</v>
       </c>
       <c r="B68" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C68" s="6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D68" s="6">
         <v>2.5</v>
       </c>
       <c r="E68" s="6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>18</v>
@@ -1869,16 +1875,16 @@
         <v>11</v>
       </c>
       <c r="B69" s="6">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C69" s="6">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D69" s="6">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
       <c r="E69" s="6">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>18</v>
@@ -1889,16 +1895,16 @@
         <v>11</v>
       </c>
       <c r="B70" s="6">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C70" s="6">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D70" s="6">
-        <v>3.3</v>
+        <v>0.8</v>
       </c>
       <c r="E70" s="6">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>18</v>
@@ -1909,16 +1915,16 @@
         <v>11</v>
       </c>
       <c r="B71" s="6">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C71" s="6">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D71" s="6">
-        <v>3.7</v>
+        <v>3.3</v>
       </c>
       <c r="E71" s="6">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>18</v>
@@ -1929,39 +1935,39 @@
         <v>11</v>
       </c>
       <c r="B72" s="6">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C72" s="6">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D72" s="6">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="E72" s="6">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="5">
+      <c r="A73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="6">
         <v>2020</v>
       </c>
-      <c r="C73" s="5">
-        <v>59</v>
-      </c>
-      <c r="D73" s="2">
+      <c r="C73" s="6">
+        <v>71</v>
+      </c>
+      <c r="D73" s="6">
         <v>3.9</v>
       </c>
-      <c r="E73" s="5">
-        <v>59</v>
+      <c r="E73" s="6">
+        <v>71</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -1969,7 +1975,7 @@
         <v>12</v>
       </c>
       <c r="B74" s="5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C74" s="5">
         <v>59</v>
@@ -1989,16 +1995,16 @@
         <v>12</v>
       </c>
       <c r="B75" s="5">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C75" s="5">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D75" s="2">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
       <c r="E75" s="5">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>27</v>
@@ -2009,16 +2015,16 @@
         <v>12</v>
       </c>
       <c r="B76" s="5">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C76" s="5">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D76" s="2">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="E76" s="5">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>27</v>
@@ -2029,16 +2035,16 @@
         <v>12</v>
       </c>
       <c r="B77" s="5">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C77" s="5">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="D77" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="E77" s="5">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>27</v>
@@ -2049,16 +2055,16 @@
         <v>12</v>
       </c>
       <c r="B78" s="5">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C78" s="5">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D78" s="2">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="E78" s="5">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>27</v>
@@ -2069,16 +2075,16 @@
         <v>12</v>
       </c>
       <c r="B79" s="5">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C79" s="5">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D79" s="2">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="E79" s="5">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>27</v>
@@ -2089,16 +2095,16 @@
         <v>12</v>
       </c>
       <c r="B80" s="5">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C80" s="5">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D80" s="2">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="E80" s="5">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>27</v>
@@ -2109,18 +2115,38 @@
         <v>12</v>
       </c>
       <c r="B81" s="5">
+        <v>2013</v>
+      </c>
+      <c r="C81" s="5">
+        <v>51</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="E81" s="5">
+        <v>51</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="5">
         <v>2012</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>56</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D82" s="2">
         <v>2.7</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E82" s="5">
         <v>56</v>
       </c>
-      <c r="F81" s="8" t="s">
+      <c r="F82" s="8" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>